<commit_message>
feat: add setWidth, setHeight
</commit_message>
<xml_diff>
--- a/test/expected/insert_chart.xlsx
+++ b/test/expected/insert_chart.xlsx
@@ -261,10 +261,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>

<commit_message>
feat: add chart methods (#48)
* feat: add setWidth, setHeight

* feat: add chart x_axis, y_axis

* feat: add chart legend

* chore: code format

* feat: chart_legend

* feat: chart_axis

* feat: add worksheet.set_print_area

* chore: remove pub

* chore: remove chart_axis set_format

* Revert "chore: remove pub"

This reverts commit 1c9e8069e249a8357e48a2d2c61fe14360262013.
</commit_message>
<xml_diff>
--- a/test/expected/insert_chart.xlsx
+++ b/test/expected/insert_chart.xlsx
@@ -215,6 +215,24 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>x-axis</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010002"/>
@@ -230,6 +248,24 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>y-axis</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010001"/>
@@ -238,7 +274,7 @@
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -261,10 +297,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>

<commit_message>
feat: add chart marker (#77)
* feat: add chart marker

* chore: fix test

* chore: fix test
</commit_message>
<xml_diff>
--- a/test/expected/insert_chart.xlsx
+++ b/test/expected/insert_chart.xlsx
@@ -97,8 +97,7 @@
     </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:stockChart>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -106,7 +105,8 @@
             <c:v>Score 1</c:v>
           </c:tx>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
           </c:marker>
           <c:dLbls>
             <c:txPr>
@@ -186,7 +186,8 @@
             <c:v>Score 2</c:v>
           </c:tx>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="diamond"/>
+            <c:size val="10"/>
           </c:marker>
           <c:dLbls>
             <c:txPr>
@@ -259,11 +260,10 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:marker val="1"/>
         <c:axId val="50010001"/>
         <c:axId val="50010002"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:stockChart>
+      <c:dateAx>
         <c:axId val="50010001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -291,7 +291,7 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -308,9 +308,8 @@
         <c:crossAx val="50010002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-      </c:catAx>
+      </c:dateAx>
       <c:valAx>
         <c:axId val="50010002"/>
         <c:scaling>

</xml_diff>

<commit_message>
feat: add chart_series set_format
</commit_message>
<xml_diff>
--- a/test/expected/insert_chart.xlsx
+++ b/test/expected/insert_chart.xlsx
@@ -104,9 +104,23 @@
           <c:tx>
             <c:v>Score 1</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="008000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="10"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="008000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
           </c:marker>
           <c:dLbls>
             <c:txPr>
@@ -185,9 +199,23 @@
           <c:tx>
             <c:v>Score 2</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="800080"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="diamond"/>
             <c:size val="10"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="800080"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
           </c:marker>
           <c:dLbls>
             <c:txPr>

</xml_diff>

<commit_message>
chore: add chart_title overlay and layout
</commit_message>
<xml_diff>
--- a/test/expected/insert_chart.xlsx
+++ b/test/expected/insert_chart.xlsx
@@ -93,7 +93,15 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1"/>
+          <c:y val="0.1"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
       <c:layout/>

</xml_diff>